<commit_message>
Añadidas gráficas del MDG en el cruce en dos puntos
</commit_message>
<xml_diff>
--- a/informe/2puntos_2vs3.xlsx
+++ b/informe/2puntos_2vs3.xlsx
@@ -13,22 +13,30 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Hoja1!$E$10</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Hoja1!$E$11:$E$15</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Hoja1!$F$10</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Hoja1!$F$11:$F$15</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Hoja1!$I$10</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Hoja1!$I$11:$I$15</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Hoja1!$J$10</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Hoja1!$J$11:$J$15</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Hoja1!$F$10</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Hoja1!$F$11:$F$15</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Hoja1!$G$10</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Hoja1!$G$11:$G$15</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Hoja1!$H$10</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Hoja1!$H$11:$H$15</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Hoja1!$E$10</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Hoja1!$E$11:$E$15</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Hoja1!$G$10</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Hoja1!$G$11:$G$15</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Hoja1!$J$10</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Hoja1!$J$11:$J$15</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Hoja1!$G$10</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Hoja1!$G$11:$G$15</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Hoja1!$H$10</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Hoja1!$H$11:$H$15</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Hoja1!$E$10</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Hoja1!$E$11:$E$15</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Hoja1!$F$10</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Hoja1!$F$11:$F$15</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Hoja1!$H$10</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Hoja1!$E$10</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Hoja1!$E$11:$E$15</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Hoja1!$F$10</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Hoja1!$F$11:$F$15</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Hoja1!$H$11:$H$15</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Hoja1!$E$10</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Hoja1!$E$11:$E$15</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Hoja1!$F$10</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Hoja1!$F$11:$F$15</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Hoja1!$I$10</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Hoja1!$I$11:$I$15</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -134,7 +142,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -344,7 +351,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -554,7 +560,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -754,12 +759,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -775,7 +780,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-ES"/>
-              <a:t>MDG-a_21</a:t>
+              <a:t>MDG-a_23</a:t>
             </a:r>
           </a:p>
         </cx:rich>
@@ -783,10 +788,10 @@
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{AD85A4ED-B959-426A-BBA7-1BE8CC8E1EAC}">
+        <cx:series layoutId="boxWhisker" uniqueId="{02184472-B7D7-4942-8ECA-577C29AB6F95}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.8</cx:f>
               <cx:v>Elite 2</cx:v>
             </cx:txData>
           </cx:tx>
@@ -796,10 +801,10 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{FA397974-7FE1-4F17-A940-216AFD4559AC}">
+        <cx:series layoutId="boxWhisker" uniqueId="{2D0B08DC-5684-484A-BFC3-0A7505D97648}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>Elite 3</cx:v>
             </cx:txData>
           </cx:tx>
@@ -831,12 +836,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -860,11 +865,11 @@
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{4B5DC250-851B-467E-8C73-F1E60973E59D}">
+        <cx:series layoutId="boxWhisker" uniqueId="{4B899F8F-FD94-4C6E-9E63-33975F12055B}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
-              <cx:v>Elite 3</cx:v>
+              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:v>Elite 2</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="0"/>
@@ -873,11 +878,11 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{17DC4129-DC1B-4AC1-A3B7-16E23575E10E}">
+        <cx:series layoutId="boxWhisker" uniqueId="{1CDC1BEE-159E-4EAC-AD93-40068454CD4C}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.6</cx:f>
-              <cx:v>Elite 2</cx:v>
+              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:v>Elite 3</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="1"/>
@@ -908,12 +913,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -929,7 +934,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="es-ES"/>
-              <a:t>MDG-a_23</a:t>
+              <a:t>MDG-a_21</a:t>
             </a:r>
           </a:p>
         </cx:rich>
@@ -937,10 +942,10 @@
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{02184472-B7D7-4942-8ECA-577C29AB6F95}">
+        <cx:series layoutId="boxWhisker" uniqueId="{33B2BEC5-B330-47BA-83DF-A7F091FDCE5E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:f>_xlchart.v1.20</cx:f>
               <cx:v>Elite 2</cx:v>
             </cx:txData>
           </cx:tx>
@@ -950,10 +955,10 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{2D0B08DC-5684-484A-BFC3-0A7505D97648}">
+        <cx:series layoutId="boxWhisker" uniqueId="{8CA2224D-FE1F-442B-908D-77DB9480D9C5}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:f>_xlchart.v1.22</cx:f>
               <cx:v>Elite 3</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4290,22 +4295,22 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="5" name="Gráfico 4"/>
+            <xdr:cNvPr id="7" name="Gráfico 6"/>
             <xdr:cNvGraphicFramePr/>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
@@ -4358,22 +4363,22 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="6" name="Gráfico 5"/>
+            <xdr:cNvPr id="2" name="Gráfico 1"/>
             <xdr:cNvGraphicFramePr/>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
@@ -4426,22 +4431,22 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>352424</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="7" name="Gráfico 6"/>
+            <xdr:cNvPr id="3" name="Gráfico 2"/>
             <xdr:cNvGraphicFramePr/>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
@@ -4760,8 +4765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4901,10 +4906,10 @@
         <v>6</v>
       </c>
       <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" t="s">
         <v>6</v>
-      </c>
-      <c r="H10" t="s">
-        <v>7</v>
       </c>
       <c r="I10" t="s">
         <v>7</v>
@@ -4915,10 +4920,10 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E11" s="1">
+        <v>112242</v>
+      </c>
+      <c r="F11" s="1">
         <v>112586</v>
-      </c>
-      <c r="F11" s="1">
-        <v>112242</v>
       </c>
       <c r="G11" s="1">
         <v>112506</v>
@@ -4935,16 +4940,16 @@
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E12" s="1">
+        <v>112280</v>
+      </c>
+      <c r="F12" s="1">
         <v>112538</v>
       </c>
-      <c r="F12" s="1">
-        <v>112280</v>
-      </c>
       <c r="G12" s="1">
+        <v>112443</v>
+      </c>
+      <c r="H12" s="1">
         <v>112210</v>
-      </c>
-      <c r="H12" s="1">
-        <v>112443</v>
       </c>
       <c r="I12" s="1">
         <v>112497</v>
@@ -4955,16 +4960,16 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E13" s="1">
+        <v>111963</v>
+      </c>
+      <c r="F13" s="1">
         <v>112350</v>
       </c>
-      <c r="F13" s="1">
-        <v>111963</v>
-      </c>
       <c r="G13" s="1">
+        <v>112604</v>
+      </c>
+      <c r="H13" s="1">
         <v>112564</v>
-      </c>
-      <c r="H13" s="1">
-        <v>112604</v>
       </c>
       <c r="I13" s="1">
         <v>111921</v>
@@ -4975,16 +4980,16 @@
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E14" s="1">
+        <v>112012</v>
+      </c>
+      <c r="F14" s="1">
         <v>112488</v>
       </c>
-      <c r="F14" s="1">
-        <v>112012</v>
-      </c>
       <c r="G14" s="1">
+        <v>112723</v>
+      </c>
+      <c r="H14" s="1">
         <v>112444</v>
-      </c>
-      <c r="H14" s="1">
-        <v>112723</v>
       </c>
       <c r="I14" s="1">
         <v>112302</v>
@@ -4995,16 +5000,16 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E15" s="1">
+        <v>112367</v>
+      </c>
+      <c r="F15" s="1">
         <v>112420</v>
       </c>
-      <c r="F15" s="1">
-        <v>112367</v>
-      </c>
       <c r="G15" s="1">
+        <v>111886</v>
+      </c>
+      <c r="H15" s="1">
         <v>112352</v>
-      </c>
-      <c r="H15" s="1">
-        <v>111886</v>
       </c>
       <c r="I15" s="1">
         <v>112163</v>

</xml_diff>